<commit_message>
User Management Test Cases
</commit_message>
<xml_diff>
--- a/[HRM] Test Cases.xlsx
+++ b/[HRM] Test Cases.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="80">
   <si>
     <t>TestCase#</t>
   </si>
@@ -40,7 +40,7 @@
     <t>Pass/Fail</t>
   </si>
   <si>
-    <t>TC_01</t>
+    <t>TC_1</t>
   </si>
   <si>
     <t>Login</t>
@@ -100,31 +100,252 @@
     <t>TC_04</t>
   </si>
   <si>
+    <t>User Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opening User Managment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- User should be conntected to the internet
+2- User should be logged in  </t>
+  </si>
+  <si>
+    <t>1- From Admin choose User Managment 
+2- Then choose Users</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User should be redirected to this URL 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t>"https://opensource-demo.orangehrmlive.com/index.php/admin/viewSystemUsers"</t>
+    </r>
+  </si>
+  <si>
     <t>TC_05</t>
   </si>
   <si>
+    <t>Search in System Users With not Saved Users</t>
+  </si>
+  <si>
+    <t>1- In the Username field enter name that doesn't exist
+2- Choose the role 
+3- Choose employee name
+4- Choose the status
+5- Press The Search button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: Youmna
+Role: All
+Employee Name: Choose from the list </t>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t>No Records Found</t>
+    </r>
+    <r>
+      <t>"
+Message should appear</t>
+    </r>
+  </si>
+  <si>
     <t>TC_06</t>
   </si>
   <si>
+    <t>1- Leave the Username field empty
+2- Choose All in the user role 
+3- Enter Name from the dropdown list 
+4- Choose All in the Status field 
+5- Press Search 
+6- Clear the employee name field and re-enter wrong name 
+7- Press Search</t>
+  </si>
+  <si>
+    <t>Employee name1: Amaresh t
+Employee name 2: Test</t>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t>No Records Found</t>
+    </r>
+    <r>
+      <t>"
+Message should appear</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Record from previous search appears  </t>
+  </si>
+  <si>
     <t>TC_07</t>
   </si>
   <si>
+    <t xml:space="preserve">1- Leave the Username field empty
+2- Choose anything in the user role 
+3- Leave Employee name field empty
+4- Choose Disabled in the Status field 
+5- Press Search </t>
+  </si>
+  <si>
+    <t>Status: Disapled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disabled users should be displayed </t>
+  </si>
+  <si>
     <t>TC_08</t>
   </si>
   <si>
+    <t xml:space="preserve">1- Leave the Username field empty
+2- Choose anything in the user role 
+3- Leave Employee name field empty
+4- Choose Enabled in the Status field 
+5- Press Search </t>
+  </si>
+  <si>
+    <t>Status: Enabled</t>
+  </si>
+  <si>
+    <t>Enabled users should be displayed</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC_09 </t>
   </si>
   <si>
+    <t xml:space="preserve">1- Leave the Username field empty
+2- Choose Admin in the user role 
+3- Leave Employee name field empty
+4- Choose anything in the Status field 
+5- Press Search </t>
+  </si>
+  <si>
+    <t>User role: Admin</t>
+  </si>
+  <si>
+    <t>All Admin users should be displayed</t>
+  </si>
+  <si>
     <t>TC_10</t>
   </si>
   <si>
+    <t>Deleting User</t>
+  </si>
+  <si>
+    <t>1- Select the record you want to delete
+2- Press Delete</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pop-up should appear to confirm that you actually need to delete this person </t>
+  </si>
+  <si>
     <t>TC_11</t>
   </si>
   <si>
+    <t>1- Select the record you want to delete
+2- Press Delete
+3- Press OK in the pop-up</t>
+  </si>
+  <si>
+    <t>User deleted successfully should appear</t>
+  </si>
+  <si>
     <t>TC_12</t>
   </si>
   <si>
+    <t>1- Select the record you want to delete
+2- Press Delete
+3- Press Cancel in the pop-up</t>
+  </si>
+  <si>
+    <t>User shouldn't be deleted</t>
+  </si>
+  <si>
     <t>TC_13</t>
+  </si>
+  <si>
+    <t>1- Select multiple records to delete
+2- Press Delete
+3- Press Ok in the pop-up</t>
+  </si>
+  <si>
+    <t>All selected records should be deleted</t>
+  </si>
+  <si>
+    <t>TC_14</t>
+  </si>
+  <si>
+    <t>Adding Users</t>
+  </si>
+  <si>
+    <t>1- Choose Add 
+2- Choose role (ESS) 
+3- Enter employee name
+4- Enter valid user name &gt;= 5 chars
+5- Choose the status 
+6- Enter password &gt;=8 chars
+7- Enter password confirmation
+8- Press Save</t>
+  </si>
+  <si>
+    <t>Role: ESS
+Emp name: From dropdown list 
+User name: Test1234
+Status: Enabled 
+Password: 12345678</t>
+  </si>
+  <si>
+    <t>User should be saved successfully and should appear in the users' list</t>
+  </si>
+  <si>
+    <t>TC_15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- Choose Add 
+2- Choose role (ESS) 
+3- Leave employee name empty </t>
+  </si>
+  <si>
+    <t>Role: ESS
+Emp name: leave it empty</t>
+  </si>
+  <si>
+    <t>Field is required should appear under the employee name field</t>
+  </si>
+  <si>
+    <t>TC_16</t>
+  </si>
+  <si>
+    <t>1- Choose Add 
+2- Choose role (ESS) 
+3- Enter employee name
+4- Enter already existed user name</t>
+  </si>
+  <si>
+    <t>Role: ESS
+Emp name: From dropdown list 
+User name: Test1234</t>
+  </si>
+  <si>
+    <t>Already exists should appear</t>
   </si>
 </sst>
 </file>
@@ -166,23 +387,29 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -211,10 +438,10 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="8.86"/>
-    <col customWidth="1" min="4" max="4" width="38.71"/>
-    <col customWidth="1" min="5" max="5" width="29.0"/>
+    <col customWidth="1" min="4" max="4" width="37.0"/>
+    <col customWidth="1" min="5" max="5" width="26.14"/>
     <col customWidth="1" min="6" max="6" width="18.86"/>
-    <col customWidth="1" min="7" max="7" width="21.29"/>
+    <col customWidth="1" min="7" max="7" width="26.57"/>
     <col customWidth="1" min="8" max="8" width="18.0"/>
   </cols>
   <sheetData>
@@ -231,7 +458,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -248,202 +475,301 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+      <c r="B5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="A6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="A7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="6"/>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="A8" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+      <c r="A9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+      <c r="A10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="A11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="A12" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="A13" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="A14" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="7">
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="D2:D4"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D5:D17"/>
+    <mergeCell ref="B5:B17"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>